<commit_message>
Logo, Search is not ready
</commit_message>
<xml_diff>
--- a/Áreas y Categorías NAS.xlsx
+++ b/Áreas y Categorías NAS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManlioniBoss\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ART</t>
   </si>
@@ -39,22 +39,10 @@
     <t>Audio</t>
   </si>
   <si>
-    <t>COM</t>
-  </si>
-  <si>
     <t>Comunidad Universitaria</t>
   </si>
   <si>
-    <t>EBO</t>
-  </si>
-  <si>
-    <t>Ebooks</t>
-  </si>
-  <si>
     <t>LIB</t>
-  </si>
-  <si>
-    <t>Libros</t>
   </si>
   <si>
     <t>VID</t>
@@ -63,67 +51,34 @@
     <t>Videos</t>
   </si>
   <si>
-    <t>humanista</t>
+    <t>Arte, Arquitectura y Diseño</t>
   </si>
   <si>
-    <t>naturaleza</t>
+    <t>Ciencias Biológicas y agropecuarias</t>
   </si>
   <si>
-    <t>ciencias físicas</t>
+    <t>Ciencias Económico-administrativas</t>
   </si>
   <si>
-    <t>ciencias bioquímicas</t>
+    <t>Ciencias exactas e ingenierías</t>
   </si>
   <si>
-    <t>ciencias química inorgánica</t>
+    <t xml:space="preserve">Ciencias de la salud </t>
   </si>
   <si>
-    <t>ciencias biológicas</t>
+    <t>Ciencias sociales y humanidades</t>
   </si>
   <si>
-    <t>ciencias matemáticas</t>
+    <t>Lenguas Extranjeras</t>
   </si>
   <si>
-    <t>expresión artística</t>
+    <t>Documentos PDF</t>
   </si>
   <si>
-    <t>comunicación</t>
+    <t>IMG</t>
   </si>
   <si>
-    <t>lenguaje</t>
-  </si>
-  <si>
-    <t>servicio</t>
-  </si>
-  <si>
-    <t>tecnología</t>
-  </si>
-  <si>
-    <t>ubicación espacial</t>
-  </si>
-  <si>
-    <t>organización</t>
-  </si>
-  <si>
-    <t>actividad física</t>
-  </si>
-  <si>
-    <t>sociabilidad</t>
-  </si>
-  <si>
-    <t>uniformados</t>
-  </si>
-  <si>
-    <t>lúdico</t>
-  </si>
-  <si>
-    <t>manualidad u operatividad</t>
-  </si>
-  <si>
-    <t>producción</t>
-  </si>
-  <si>
-    <t>urbano</t>
+    <t>Imágenes y Diagramas</t>
   </si>
 </sst>
 </file>
@@ -1591,13 +1546,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1648,13 +1603,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1705,13 +1660,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1762,13 +1717,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1819,13 +1774,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1876,13 +1831,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1933,13 +1888,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1990,13 +1945,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2047,13 +2002,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2104,13 +2059,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2161,13 +2116,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2218,13 +2173,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2275,13 +2230,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2332,13 +2287,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2389,13 +2344,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2446,13 +2401,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2503,13 +2458,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2560,13 +2515,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2617,13 +2572,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2674,13 +2629,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2731,13 +2686,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2788,13 +2743,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2845,13 +2800,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2902,13 +2857,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2959,13 +2914,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3016,13 +2971,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3073,13 +3028,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3130,13 +3085,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3187,13 +3142,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3244,13 +3199,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3301,13 +3256,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3358,13 +3313,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3415,13 +3370,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3472,13 +3427,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3529,13 +3484,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3586,13 +3541,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3643,13 +3598,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3700,13 +3655,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3757,13 +3712,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4332,13 +4287,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4389,13 +4344,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4446,13 +4401,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4503,13 +4458,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4560,13 +4515,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4617,13 +4572,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4674,13 +4629,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4731,13 +4686,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4788,13 +4743,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5263,7 +5218,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -5271,175 +5226,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>14</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>16</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>18</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="51" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>20</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5451,10 +5302,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5463,7 +5314,7 @@
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5479,36 +5330,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
+      <c r="A5" t="s">
+        <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
+      <c r="B5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>